<commit_message>
fully added refs merge and generating result mart
</commit_message>
<xml_diff>
--- a/input_files/refs/demo1/Справочник отчетных показателей.xlsx
+++ b/input_files/refs/demo1/Справочник отчетных показателей.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bitoche\REPOS\USER\dissertation_project\input_files\refs\demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7111A4-928D-47FB-849D-223BC8625D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDCEFC-C12A-4FE0-828A-AB50FF965C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>effective_from_dttm</t>
   </si>
@@ -37,13 +37,91 @@
   </si>
   <si>
     <t>report_item_name</t>
+  </si>
+  <si>
+    <t>RES_RA_AMT_METRICS</t>
+  </si>
+  <si>
+    <t>PV_TOTAL_METRICS</t>
+  </si>
+  <si>
+    <t>obligations_lrc_METRICS</t>
+  </si>
+  <si>
+    <t>RES_LS_METRICS</t>
+  </si>
+  <si>
+    <t>RES_CSM_METRICS</t>
+  </si>
+  <si>
+    <t>RES_RA_L_AMT_METRICS</t>
+  </si>
+  <si>
+    <t>PV_L_TOTAL_METRICS</t>
+  </si>
+  <si>
+    <t>OBLIG_OOCHP_METRICS</t>
+  </si>
+  <si>
+    <t>OBLIG_OVT_METRICS</t>
+  </si>
+  <si>
+    <t>ACTIVE_AQUIS_METRICS</t>
+  </si>
+  <si>
+    <t>ANOTHER_METRICS</t>
+  </si>
+  <si>
+    <t>SUMM_METRICS</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>amt</t>
+  </si>
+  <si>
+    <t>рисковая поправка на нефинансовый риск</t>
+  </si>
+  <si>
+    <t>оценка приведенной стоимости будущих денежных потоков</t>
+  </si>
+  <si>
+    <t>обязательства, оцененные с использованием подхода на основе распределения премии</t>
+  </si>
+  <si>
+    <t>Компонент убытка</t>
+  </si>
+  <si>
+    <t>маржа за предусмотренные договором услуги</t>
+  </si>
+  <si>
+    <t>рисковая поправка по возникшим требованиям</t>
+  </si>
+  <si>
+    <t>приведенная стоимость потоков по возникшим требованиям</t>
+  </si>
+  <si>
+    <t>Обязательства по оставшейся части покрытия, кроме компонента убытка</t>
+  </si>
+  <si>
+    <t>Обязательства по возникшим требованиям</t>
+  </si>
+  <si>
+    <t>Активы, признанные в отношении аквизиционных денежных потоков</t>
+  </si>
+  <si>
+    <t>Прочее</t>
+  </si>
+  <si>
+    <t>Итого</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +134,12 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -72,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -95,17 +179,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -386,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,170 +521,227 @@
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3">
-        <v>1</v>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D3" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D6" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D7" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D8" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D10" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D12" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>401404</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
         <v>401404</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added ref cleanup settings added rep PL started work at struct cols.
</commit_message>
<xml_diff>
--- a/input_files/refs/demo1/Справочник отчетных показателей.xlsx
+++ b/input_files/refs/demo1/Справочник отчетных показателей.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bitoche\REPOS\USER\dissertation_project\input_files\refs\demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFDCEFC-C12A-4FE0-828A-AB50FF965C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E7E88F-71F1-46F2-8454-48C95A6664CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>effective_from_dttm</t>
   </si>
@@ -115,6 +115,159 @@
   </si>
   <si>
     <t>Итого</t>
+  </si>
+  <si>
+    <t>изменение величины обязательств по возникшим требованиям</t>
+  </si>
+  <si>
+    <t>CLAIMS_OBLIGAT_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Изменения величины обязательств по возникшим требованиям</t>
+  </si>
+  <si>
+    <t>CLAIMS_OBLIGAT_OSBU_PL</t>
+  </si>
+  <si>
+    <t>расходы по услугам страхования, понесенные в течение отчетного периода, не отнесенные к компоненту убытка</t>
+  </si>
+  <si>
+    <t>EXP_LOSS_INS_OSBU_PL</t>
+  </si>
+  <si>
+    <t>Финансовые расходы (доходы) по группам договоров страхования и выпущенных (принятых) договоров перестрахования</t>
+  </si>
+  <si>
+    <t>FIN_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Результат оказания страховых услуг по группам договоров страхования и выпущенных (принятых) договоров перестрахования</t>
+  </si>
+  <si>
+    <t>FIN_RES_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>возникшие страховые убытки и прочие расходы по требованиям</t>
+  </si>
+  <si>
+    <t>INSHUR_LOSSES_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Возникшие страховые убытки и прочие расходы по требованиям</t>
+  </si>
+  <si>
+    <t>INSHUR_LOSSES_OSBU_PL</t>
+  </si>
+  <si>
+    <t>Инвестиционный доход</t>
+  </si>
+  <si>
+    <t>INV_GROSS_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Расходы по страхованию по группам договоров страхования и выпущенных (принятых) договоров перестрахования, в том числе:</t>
+  </si>
+  <si>
+    <t>LOSS_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>убытки и восстановление убытков по группам обременительных договоров</t>
+  </si>
+  <si>
+    <t>LOSSES_OBREM_CONTR_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Убытки и восстановление убытков по группам обременительных договоров</t>
+  </si>
+  <si>
+    <t>LOSSES_OBREM_CONTR_OSBU_PL</t>
+  </si>
+  <si>
+    <t>прочее</t>
+  </si>
+  <si>
+    <t>OTHER_OSBU_PL</t>
+  </si>
+  <si>
+    <t>изменение рисковой поправки на нефинансовый риск, не отнесенное к компоненту убытка</t>
+  </si>
+  <si>
+    <t>RA_RELEASE_N_OSBU_PL</t>
+  </si>
+  <si>
+    <t>сумма маржи за предусмотренные договором услуги, признанной в составе прибыли или убытка вследствие предоставления услуг по договору страхования в отчетном периоде</t>
+  </si>
+  <si>
+    <t>RELEASE_CSM_PERIOD_OSBU_PL</t>
+  </si>
+  <si>
+    <t>Страховые расходы (Аморт аквизы)</t>
+  </si>
+  <si>
+    <t>RES_ACQ_AMORT</t>
+  </si>
+  <si>
+    <t>амортизация аквизиционных денежных потоков</t>
+  </si>
+  <si>
+    <t>RES_ACQ_AMORT_LOSSES_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Амортизация аквизиционных денежных потоков</t>
+  </si>
+  <si>
+    <t>RES_ACQ_AMORT_LOSSES_OSBU_PL</t>
+  </si>
+  <si>
+    <t>суммы, относящиеся к аквизиционным денежным потокам</t>
+  </si>
+  <si>
+    <t>RES_ACQ_AMORT_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>Суммы, относящиеся к аквизиционным денежным потокам</t>
+  </si>
+  <si>
+    <t>RES_ACQ_AMORT_OSBU_PL</t>
+  </si>
+  <si>
+    <t>выручка по страхованию по договорам страхования, оцениваемым с применением подхода на основе распределения премии</t>
+  </si>
+  <si>
+    <t>REV_OSBU_PL</t>
+  </si>
+  <si>
+    <t>суммы, связанные с оказанием услуг</t>
+  </si>
+  <si>
+    <t>SUM_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Суммы, связанные с оказанием услуг, в том числе:                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                            </t>
+  </si>
+  <si>
+    <t>SUM_OSBU_PL</t>
+  </si>
+  <si>
+    <t>Итого Расходы</t>
+  </si>
+  <si>
+    <t>TOTAL_LOSSES_OSBU_PL</t>
+  </si>
+  <si>
+    <t>Итого Выручка</t>
+  </si>
+  <si>
+    <t>TOTAL_REV_OSBU_PL</t>
+  </si>
+  <si>
+    <t>Выручка по страхованию по группам договоров страхования и выпущенных (принятых) договоров перестрахования, в том числе:</t>
+  </si>
+  <si>
+    <t>VR_OSBU_B_PL</t>
+  </si>
+  <si>
+    <t>pl</t>
   </si>
 </sst>
 </file>
@@ -156,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -207,11 +360,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -227,7 +393,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,19 +900,444 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
         <v>401404</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added liab_analysis report added ref_approach upd in main: - added method to save df to excel - added debug-saving all dfs to out excel file - changed "where condition" for ref_report_items ref -- now its take only current report entries
</commit_message>
<xml_diff>
--- a/input_files/refs/demo1/Справочник отчетных показателей.xlsx
+++ b/input_files/refs/demo1/Справочник отчетных показателей.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bitoche\REPOS\USER\dissertation_project\input_files\refs\demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB876E0D-9B72-4CC3-A576-268F7B5DC45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3126508-9F0C-4ECE-B15D-C1523BA74AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="162">
   <si>
     <t>effective_from_dttm</t>
   </si>
@@ -483,6 +483,45 @@
   </si>
   <si>
     <t>Русское наименование SUM_CR</t>
+  </si>
+  <si>
+    <t>REVENUE_INSHUR</t>
+  </si>
+  <si>
+    <t>DEPREC_AQUIS_CF</t>
+  </si>
+  <si>
+    <t>CHANGE_OBLIGATE</t>
+  </si>
+  <si>
+    <t>AHOTHER_COST_INSHUR</t>
+  </si>
+  <si>
+    <t>COST_INSHUR</t>
+  </si>
+  <si>
+    <t>FIN_RES</t>
+  </si>
+  <si>
+    <t>Русское наименование REVENUE_INSHUR</t>
+  </si>
+  <si>
+    <t>Русское наименование DEPREC_AQUIS_CF</t>
+  </si>
+  <si>
+    <t>Русское наименование CHANGE_OBLIGATE</t>
+  </si>
+  <si>
+    <t>Русское наименование AHOTHER_COST_INSHUR</t>
+  </si>
+  <si>
+    <t>Русское наименование COST_INSHUR</t>
+  </si>
+  <si>
+    <t>Русское наименование FIN_RES</t>
+  </si>
+  <si>
+    <t>liab_analysis</t>
   </si>
 </sst>
 </file>
@@ -790,7 +829,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -879,13 +918,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -894,47 +930,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1218,17 +1242,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" style="34" customWidth="1"/>
     <col min="4" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1236,10 +1260,10 @@
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -2287,155 +2311,529 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="B63" s="38" t="s">
+      <c r="B63" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="C63" s="39" t="s">
+      <c r="C63" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D63" s="40">
-        <v>1</v>
-      </c>
-      <c r="E63" s="41">
+      <c r="D63" s="11">
+        <v>1</v>
+      </c>
+      <c r="E63" s="12">
         <v>401404</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="42" t="s">
+      <c r="A64" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B64" s="32" t="s">
+      <c r="B64" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D64" s="30">
-        <v>1</v>
-      </c>
-      <c r="E64" s="43">
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="42" t="s">
+      <c r="A65" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B65" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="30">
-        <v>1</v>
-      </c>
-      <c r="E65" s="43">
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="42" t="s">
+      <c r="A66" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="32" t="s">
+      <c r="B66" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="30">
-        <v>1</v>
-      </c>
-      <c r="E66" s="43">
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="42" t="s">
+      <c r="A67" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B67" s="32" t="s">
+      <c r="B67" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D67" s="30">
-        <v>1</v>
-      </c>
-      <c r="E67" s="43">
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="42" t="s">
+      <c r="A68" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B68" s="32" t="s">
+      <c r="B68" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C68" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="30">
-        <v>1</v>
-      </c>
-      <c r="E68" s="43">
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="42" t="s">
+      <c r="A69" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="32" t="s">
+      <c r="B69" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C69" s="35" t="s">
+      <c r="C69" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="30">
-        <v>1</v>
-      </c>
-      <c r="E69" s="43">
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="42" t="s">
+      <c r="A70" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="35" t="s">
+      <c r="C70" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="30">
-        <v>1</v>
-      </c>
-      <c r="E70" s="43">
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+      <c r="E70" s="14">
         <v>401404</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="44" t="s">
+      <c r="A71" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="45" t="s">
+      <c r="B71" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="46" t="s">
+      <c r="C71" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="D71" s="47">
-        <v>1</v>
-      </c>
-      <c r="E71" s="48">
+      <c r="D71" s="28">
+        <v>1</v>
+      </c>
+      <c r="E71" s="29">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B72" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="11">
+        <v>1</v>
+      </c>
+      <c r="E72" s="12">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B73" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
+      <c r="E79" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B83" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B85" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B86" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+      <c r="E86" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B87" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1</v>
+      </c>
+      <c r="E88" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B89" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B90" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B91" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
+      <c r="E91" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B92" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
+      <c r="E92" s="14">
+        <v>401404</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B93" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C93" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D93" s="18">
+        <v>1</v>
+      </c>
+      <c r="E93" s="19">
         <v>401404</v>
       </c>
     </row>

</xml_diff>